<commit_message>
Working on the slides for the master seminar
</commit_message>
<xml_diff>
--- a/IR-Praesentation/ExampleHITS.xlsx
+++ b/IR-Praesentation/ExampleHITS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="150" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -689,9 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:Y48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2065,10 +2063,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.0236220472440944" bottom="1.0236220472440944" header="0.78740157480314965" footer="0.78740157480314965"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddHeader>&amp;CBeispiel, Tikhoncheva 2015, berechnet in Excel 2007</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
@@ -2078,7 +2076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>